<commit_message>
had to modify some column names in coho populations file to ease things
</commit_message>
<xml_diff>
--- a/data/coho_populations/coho_populations.xlsx
+++ b/data/coho_populations/coho_populations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverFishStatus\data\coho_populations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710E3625-3B35-426F-A88E-6E51FA4036B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A614CB73-35F6-4CD2-B43E-8F1F0039E5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="46">
   <si>
     <t>spawn_site</t>
   </si>
@@ -33,12 +33,6 @@
     <t>coho_TRT_POPID</t>
   </si>
   <si>
-    <t>MPG</t>
-  </si>
-  <si>
-    <t>POP_NAME</t>
-  </si>
-  <si>
     <t>ACM</t>
   </si>
   <si>
@@ -157,6 +151,18 @@
   </si>
   <si>
     <t>Clearwater River</t>
+  </si>
+  <si>
+    <t>coho_MPG</t>
+  </si>
+  <si>
+    <t>coho_POP_NAME</t>
+  </si>
+  <si>
+    <t>Snake River Coho Salmon</t>
+  </si>
+  <si>
+    <t>coho_ESU_DPS</t>
   </si>
 </sst>
 </file>
@@ -474,332 +480,398 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
         <v>39</v>
       </c>
-      <c r="C16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
         <v>39</v>
       </c>
-      <c r="C17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" t="s">
         <v>39</v>
       </c>
-      <c r="C18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
         <v>7</v>
       </c>
-      <c r="B21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D22">
-    <sortCondition ref="C2:C22"/>
-    <sortCondition ref="B2:B22"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E22">
+    <sortCondition ref="D2:D22"/>
     <sortCondition ref="A2:A22"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added LOSTIW to coho_populations.xlsx
</commit_message>
<xml_diff>
--- a/data/coho_populations/coho_populations.xlsx
+++ b/data/coho_populations/coho_populations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverFishStatus\data\coho_populations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5BE03A-3B9C-462C-87AA-5F683784CFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648880EA-53F8-478E-97E3-2C3EC9BAEE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="46">
-  <si>
-    <t>spawn_site</t>
-  </si>
-  <si>
-    <t>coho_TRT_POPID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="47">
   <si>
     <t>ACM</t>
   </si>
@@ -153,16 +147,25 @@
     <t>Clearwater River</t>
   </si>
   <si>
-    <t>coho_MPG</t>
-  </si>
-  <si>
-    <t>coho_POP_NAME</t>
-  </si>
-  <si>
     <t>Snake River Coho Salmon</t>
   </si>
   <si>
-    <t>coho_ESU_DPS</t>
+    <t>LOSTIW</t>
+  </si>
+  <si>
+    <t>site_code</t>
+  </si>
+  <si>
+    <t>coho_mpg</t>
+  </si>
+  <si>
+    <t>coho_esu_dps</t>
+  </si>
+  <si>
+    <t>coho_popid</t>
+  </si>
+  <si>
+    <t>coho_popname</t>
   </si>
 </sst>
 </file>
@@ -480,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -497,382 +500,399 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
         <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
         <v>21</v>
-      </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
         <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
         <v>31</v>
-      </c>
-      <c r="E11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
         <v>31</v>
-      </c>
-      <c r="E12" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
         <v>31</v>
-      </c>
-      <c r="E13" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
         <v>29</v>
       </c>
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>31</v>
-      </c>
-      <c r="E14" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
         <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
         <v>35</v>
       </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" t="s">
-        <v>37</v>
-      </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" t="s">
         <v>36</v>
-      </c>
-      <c r="B18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
         <v>5</v>
-      </c>
-      <c r="B21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
         <v>4</v>
       </c>
-      <c r="B22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" t="s">
-        <v>6</v>
-      </c>
       <c r="E22" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E22">
-    <sortCondition ref="D2:D22"/>
-    <sortCondition ref="A2:A22"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E23">
+    <sortCondition ref="D2:D23"/>
+    <sortCondition ref="A2:A23"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updating site/node maps; cleaning up figures
</commit_message>
<xml_diff>
--- a/data/coho_populations/coho_populations.xlsx
+++ b/data/coho_populations/coho_populations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverFishStatus\data\coho_populations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648880EA-53F8-478E-97E3-2C3EC9BAEE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F141BF64-F109-4280-8EC8-8EF947436D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
added COU to configuration files
</commit_message>
<xml_diff>
--- a/data/coho_populations/coho_populations.xlsx
+++ b/data/coho_populations/coho_populations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverFishStatus\data\coho_populations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F141BF64-F109-4280-8EC8-8EF947436D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05609EC6-3254-469F-9911-65ED4F56A202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="48">
   <si>
     <t>ACM</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>coho_popname</t>
+  </si>
+  <si>
+    <t>CLC</t>
   </si>
 </sst>
 </file>
@@ -483,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -738,24 +741,24 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
         <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
         <v>40</v>
@@ -764,15 +767,15 @@
         <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
         <v>40</v>
@@ -789,7 +792,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
         <v>40</v>
@@ -806,7 +809,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
         <v>40</v>
@@ -823,24 +826,24 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
         <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="E20" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
         <v>40</v>
@@ -857,7 +860,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B22" t="s">
         <v>40</v>
@@ -874,7 +877,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B23" t="s">
         <v>40</v>
@@ -889,10 +892,27 @@
         <v>5</v>
       </c>
     </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E23">
-    <sortCondition ref="D2:D23"/>
-    <sortCondition ref="A2:A23"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E24">
+    <sortCondition ref="D2:D24"/>
+    <sortCondition ref="A2:A24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated coho populations file based on sy24 detections
</commit_message>
<xml_diff>
--- a/data/coho_populations/coho_populations.xlsx
+++ b/data/coho_populations/coho_populations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverFishStatus\data\coho_populations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05609EC6-3254-469F-9911-65ED4F56A202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1600B57-AEE1-4ECD-A7C5-DBC3FD764876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="58">
   <si>
     <t>ACM</t>
   </si>
@@ -169,6 +169,36 @@
   </si>
   <si>
     <t>CLC</t>
+  </si>
+  <si>
+    <t>LTR</t>
+  </si>
+  <si>
+    <t>MTR</t>
+  </si>
+  <si>
+    <t>UTR</t>
+  </si>
+  <si>
+    <t>TFH</t>
+  </si>
+  <si>
+    <t>TPJ</t>
+  </si>
+  <si>
+    <t>SNTUC-c</t>
+  </si>
+  <si>
+    <t>Tucannon River</t>
+  </si>
+  <si>
+    <t>WEN</t>
+  </si>
+  <si>
+    <t>GRWEN-c</t>
+  </si>
+  <si>
+    <t>Wenaha River</t>
   </si>
 </sst>
 </file>
@@ -486,22 +516,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -518,7 +548,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -535,7 +565,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -552,7 +582,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -569,7 +599,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -586,7 +616,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -603,7 +633,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -620,7 +650,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -637,7 +667,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -654,7 +684,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -671,7 +701,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -688,7 +718,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -705,7 +735,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -722,7 +752,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -739,7 +769,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -756,7 +786,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -773,7 +803,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -790,7 +820,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -807,7 +837,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -824,7 +854,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -841,26 +871,26 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>0</v>
       </c>
       <c r="B22" t="s">
         <v>40</v>
@@ -875,9 +905,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B23" t="s">
         <v>40</v>
@@ -892,9 +922,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B24" t="s">
         <v>40</v>
@@ -909,10 +939,112 @@
         <v>5</v>
       </c>
     </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E24">
-    <sortCondition ref="D2:D24"/>
-    <sortCondition ref="A2:A24"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E25">
+    <sortCondition ref="D2:D25"/>
+    <sortCondition ref="A2:A25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>